<commit_message>
Added BTC change to influcence buy/sell
</commit_message>
<xml_diff>
--- a/backtest results/Backtest .xlsx
+++ b/backtest results/Backtest .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25120" windowHeight="8740" tabRatio="500"/>
+    <workbookView xWindow="4880" yWindow="2400" windowWidth="25120" windowHeight="8740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,11 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,6 +441,14 @@
         <v>2.7834464000000003</v>
       </c>
     </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>42941</v>
+      </c>
+      <c r="B3">
+        <v>1.8118E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
seperated btc and eth trades
</commit_message>
<xml_diff>
--- a/backtest results/Backtest .xlsx
+++ b/backtest results/Backtest .xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>-0.00004788</t>
+  </si>
+  <si>
+    <t>1 BTC price</t>
+  </si>
+  <si>
+    <t>7/26/2017 part 2</t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -378,7 +384,7 @@
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,10 +398,13 @@
         <v>3</v>
       </c>
       <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42939</v>
       </c>
@@ -436,17 +445,129 @@
       <c r="Q2" t="s">
         <v>4</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <f>P2*2779</f>
         <v>2.7834464000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>42941</v>
-      </c>
-      <c r="B3">
-        <v>1.8118E-4</v>
+        <v>42942</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.4610000000000001E-5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-4.8180000000000003E-5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.9999999998100003E-8</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.9999999998100003E-8</v>
+      </c>
+      <c r="H3">
+        <v>-1.0001E-4</v>
+      </c>
+      <c r="I3">
+        <v>-2.9503999999999999E-4</v>
+      </c>
+      <c r="J3" s="2">
+        <v>9.2159999999999999E-5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-9.2180000000000002E-5</v>
+      </c>
+      <c r="P3" s="2">
+        <f>SUM(B3:L3)</f>
+        <v>-3.2858000000000377E-4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>2470</v>
+      </c>
+      <c r="S3" s="2">
+        <f>P3*R3</f>
+        <v>-0.81159260000000932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1.2284000000000001E-4</v>
+      </c>
+      <c r="P4">
+        <f>SUM(B4:O4)</f>
+        <v>1.2284000000000001E-4</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4">
+        <v>2552</v>
+      </c>
+      <c r="S4">
+        <f>P4*R4</f>
+        <v>0.31348768000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>42943</v>
+      </c>
+      <c r="B5">
+        <v>-1.7384E-4</v>
+      </c>
+      <c r="C5">
+        <v>1.2310000000000001E-4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.6820000000000002E-5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.0000000003400001E-8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.0000000003400001E-8</v>
+      </c>
+      <c r="G5">
+        <v>1.9646E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>-1.4000000001E-7</v>
+      </c>
+      <c r="I5">
+        <v>5.8022E-4</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.9769999999999999E-5</v>
+      </c>
+      <c r="K5">
+        <v>-1.1587E-4</v>
+      </c>
+      <c r="P5">
+        <f>SUM(B5:L5)</f>
+        <v>6.4655999999999676E-4</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>2567</v>
+      </c>
+      <c r="S5">
+        <f>P5*R5</f>
+        <v>1.6597195199999917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added price into tweepy query
</commit_message>
<xml_diff>
--- a/backtest results/Backtest .xlsx
+++ b/backtest results/Backtest .xlsx
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,6 +573,25 @@
         <v>1.6080971499999916</v>
       </c>
     </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>42945</v>
+      </c>
+      <c r="B6">
+        <v>6.5136999999999997E-4</v>
+      </c>
+      <c r="P6">
+        <f>SUM(B6:L6)</f>
+        <v>6.5136999999999997E-4</v>
+      </c>
+      <c r="R6">
+        <v>2677</v>
+      </c>
+      <c r="S6">
+        <f>P6*R6</f>
+        <v>1.7437174899999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>